<commit_message>
summery error report excel format added
</commit_message>
<xml_diff>
--- a/Input/Input_Dcoe.xlsx
+++ b/Input/Input_Dcoe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPath\Bot-A-Thon\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPath\Team-IESians (Abhishek kumar kushwaha, 8305238599)\Bot-A-Thon\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7A2925-8BDC-4D0D-A5D3-7BBB895D494E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782F6156-4DE0-45B1-BB4A-D7C66F2DAF71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2475" yWindow="3660" windowWidth="21600" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
   <si>
     <t>S. No.</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>pat1.khata@gmail.com</t>
+  </si>
+  <si>
+    <t>pat1.khata@gmail</t>
   </si>
 </sst>
 </file>
@@ -485,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -920,7 +923,7 @@
         <v>2021</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
status-SUCCESS/FAIL add and getPassword Email used
</commit_message>
<xml_diff>
--- a/Input/Input_Dcoe.xlsx
+++ b/Input/Input_Dcoe.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPath\Team-IESians (Abhishek kumar kushwaha, 8305238599)\Bot-A-Thon\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPath\Team-IESians (Abhishek kumar kushwaha, 8305238599)\Bot-A-Thon 1.0\Bot-A-Thon\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782F6156-4DE0-45B1-BB4A-D7C66F2DAF71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF90DBAB-664D-4F77-A707-F8CA85FBD66B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2475" yWindow="3660" windowWidth="21600" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5925" yWindow="2310" windowWidth="21600" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,9 +43,6 @@
     <t>BHAVYA ANAND</t>
   </si>
   <si>
-    <t>20MC2C029</t>
-  </si>
-  <si>
     <t>MCA</t>
   </si>
   <si>
@@ -202,6 +199,9 @@
   </si>
   <si>
     <t>pat1.khata@gmail</t>
+  </si>
+  <si>
+    <t>20MC2C029</t>
   </si>
 </sst>
 </file>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -523,7 +523,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -534,16 +534,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="2">
         <v>2021</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -551,19 +551,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="2">
         <v>2021</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -571,19 +571,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="2">
         <v>2021</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -591,19 +591,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" s="2">
         <v>2021</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -611,19 +611,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="2">
         <v>2021</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -631,19 +631,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="E7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="2">
         <v>2021</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -651,19 +651,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="2">
         <v>2021</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -671,19 +671,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F9" s="2">
         <v>2021</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -691,19 +691,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F10" s="2">
         <v>2021</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -711,19 +711,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" s="2">
         <v>2021</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -731,19 +731,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="E12" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F12" s="4">
         <v>2021</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -751,19 +751,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F13" s="4">
         <v>2021</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -771,19 +771,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="E14" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14" s="4">
         <v>2021</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -791,19 +791,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="E15" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F15" s="4">
         <v>2021</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -811,19 +811,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="E16" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F16" s="4">
         <v>2021</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -831,19 +831,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="E17" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F17" s="4">
         <v>2021</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -851,19 +851,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="E18" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F18" s="4">
         <v>2021</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -871,19 +871,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="E19" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F19" s="4">
         <v>2021</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -891,19 +891,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="E20" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F20" s="4">
         <v>2021</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -911,19 +911,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F21" s="4">
         <v>2021</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -931,19 +931,19 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F22">
         <v>2023</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -951,13 +951,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
         <v>51</v>
       </c>
-      <c r="C23" t="s">
-        <v>52</v>
-      </c>
       <c r="E23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F23">
         <v>2023</v>
@@ -968,19 +968,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F24">
         <v>2023</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1970,19 +1970,19 @@
     <hyperlink ref="G5" r:id="rId7" xr:uid="{3649D93F-0175-4604-A876-B76F1964BD06}"/>
     <hyperlink ref="G6" r:id="rId8" xr:uid="{6DD12101-AE8C-4A77-AFAE-F1D984064F7B}"/>
     <hyperlink ref="G8" r:id="rId9" xr:uid="{D26E9973-57DA-48A2-9BEA-094393C1D2DF}"/>
-    <hyperlink ref="G9" r:id="rId10" xr:uid="{5BD92786-8B10-4AE6-B63B-423BAB404857}"/>
-    <hyperlink ref="G10" r:id="rId11" xr:uid="{9C0128BD-5864-4A56-B533-CD9F1649C1AE}"/>
-    <hyperlink ref="G13" r:id="rId12" xr:uid="{0B3A7450-3C4F-4DCC-AAC1-FEB0BE8E60D2}"/>
-    <hyperlink ref="G15" r:id="rId13" xr:uid="{A9FABE30-2381-48F3-A505-113CA9E977C9}"/>
-    <hyperlink ref="G16" r:id="rId14" xr:uid="{9C422A06-C99F-4B2A-AACF-4538F64B8427}"/>
-    <hyperlink ref="G18" r:id="rId15" xr:uid="{26585250-A291-41EC-BC3F-94A451228068}"/>
-    <hyperlink ref="G21" r:id="rId16" xr:uid="{E9A73B9B-9FDA-486B-B511-F42B8B141875}"/>
-    <hyperlink ref="G19" r:id="rId17" xr:uid="{DCE873D3-F359-4D2C-A782-FD0640A92C3B}"/>
-    <hyperlink ref="G20" r:id="rId18" xr:uid="{4471C13D-7768-4A19-B6EC-59C4B9EB651B}"/>
-    <hyperlink ref="G17" r:id="rId19" xr:uid="{0F36E02D-7773-41FA-93C0-CFDDF0543ED5}"/>
-    <hyperlink ref="G14" r:id="rId20" xr:uid="{C72096E4-3BE1-400F-8A95-1975719D270B}"/>
-    <hyperlink ref="G12" r:id="rId21" xr:uid="{94E99EF6-A9DA-4FB3-A4F3-C1AFFE0F4814}"/>
-    <hyperlink ref="G11" r:id="rId22" xr:uid="{40821E4F-7EF0-493B-A81A-D79C94DFC845}"/>
+    <hyperlink ref="G10" r:id="rId10" xr:uid="{9C0128BD-5864-4A56-B533-CD9F1649C1AE}"/>
+    <hyperlink ref="G13" r:id="rId11" xr:uid="{0B3A7450-3C4F-4DCC-AAC1-FEB0BE8E60D2}"/>
+    <hyperlink ref="G15" r:id="rId12" xr:uid="{A9FABE30-2381-48F3-A505-113CA9E977C9}"/>
+    <hyperlink ref="G16" r:id="rId13" xr:uid="{9C422A06-C99F-4B2A-AACF-4538F64B8427}"/>
+    <hyperlink ref="G18" r:id="rId14" xr:uid="{26585250-A291-41EC-BC3F-94A451228068}"/>
+    <hyperlink ref="G21" r:id="rId15" xr:uid="{E9A73B9B-9FDA-486B-B511-F42B8B141875}"/>
+    <hyperlink ref="G19" r:id="rId16" xr:uid="{DCE873D3-F359-4D2C-A782-FD0640A92C3B}"/>
+    <hyperlink ref="G20" r:id="rId17" xr:uid="{4471C13D-7768-4A19-B6EC-59C4B9EB651B}"/>
+    <hyperlink ref="G17" r:id="rId18" xr:uid="{0F36E02D-7773-41FA-93C0-CFDDF0543ED5}"/>
+    <hyperlink ref="G14" r:id="rId19" xr:uid="{C72096E4-3BE1-400F-8A95-1975719D270B}"/>
+    <hyperlink ref="G12" r:id="rId20" xr:uid="{94E99EF6-A9DA-4FB3-A4F3-C1AFFE0F4814}"/>
+    <hyperlink ref="G11" r:id="rId21" xr:uid="{40821E4F-7EF0-493B-A81A-D79C94DFC845}"/>
+    <hyperlink ref="G9" r:id="rId22" xr:uid="{741FBF0E-C9DF-4832-95F5-67F5549715F0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>